<commit_message>
custom accuracy + 데이터 1000개
</commit_message>
<xml_diff>
--- a/DATA_goal/Junction_Flooding_1.xlsx
+++ b/DATA_goal/Junction_Flooding_1.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,14 +464,14 @@
     <col width="9" customWidth="1" min="20" max="20"/>
     <col width="8" customWidth="1" min="21" max="21"/>
     <col width="7" customWidth="1" min="22" max="22"/>
-    <col width="8" customWidth="1" min="23" max="23"/>
+    <col width="7" customWidth="1" min="23" max="23"/>
     <col width="7" customWidth="1" min="24" max="24"/>
     <col width="7" customWidth="1" min="25" max="25"/>
     <col width="8" customWidth="1" min="26" max="26"/>
     <col width="7" customWidth="1" min="27" max="27"/>
     <col width="7" customWidth="1" min="28" max="28"/>
     <col width="7" customWidth="1" min="29" max="29"/>
-    <col width="8" customWidth="1" min="30" max="30"/>
+    <col width="7" customWidth="1" min="30" max="30"/>
     <col width="7" customWidth="1" min="31" max="31"/>
     <col width="8" customWidth="1" min="32" max="32"/>
     <col width="7" customWidth="1" min="33" max="33"/>
@@ -967,207 +967,103 @@
         <v>40751.31944444445</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>11.111</v>
+        <v>11.11</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>8.584</v>
+        <v>8.58</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.268</v>
+        <v>0.27</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>24.739</v>
+        <v>24.74</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>20.357</v>
+        <v>20.36</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>8.952</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>35.271</v>
+        <v>35.27</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>14.017</v>
+        <v>14.02</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>6.416</v>
+        <v>6.42</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>9.654</v>
+        <v>9.65</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>10.284</v>
+        <v>10.28</v>
       </c>
       <c r="M5" s="4" t="n">
-        <v>10.565</v>
+        <v>10.56</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>2.899</v>
+        <v>2.9</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>8.798</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>12.832</v>
+        <v>12.83</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>7.488</v>
+        <v>7.49</v>
       </c>
       <c r="R5" s="4" t="n">
-        <v>0.159</v>
+        <v>0.16</v>
       </c>
       <c r="S5" s="4" t="n">
-        <v>0.417</v>
+        <v>0.42</v>
       </c>
       <c r="T5" s="4" t="n">
-        <v>129.861</v>
+        <v>129.86</v>
       </c>
       <c r="U5" s="4" t="n">
-        <v>25.249</v>
+        <v>25.25</v>
       </c>
       <c r="V5" s="4" t="n">
-        <v>8.218999999999999</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="W5" s="4" t="n">
-        <v>16.793</v>
+        <v>16.79</v>
       </c>
       <c r="X5" s="4" t="n">
-        <v>9.285</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="Y5" s="4" t="n">
-        <v>1.183</v>
+        <v>1.18</v>
       </c>
       <c r="Z5" s="4" t="n">
-        <v>17.258</v>
+        <v>17.26</v>
       </c>
       <c r="AA5" s="4" t="n">
-        <v>7.335</v>
+        <v>7.34</v>
       </c>
       <c r="AB5" s="4" t="n">
-        <v>6.868</v>
+        <v>6.87</v>
       </c>
       <c r="AC5" s="4" t="n">
-        <v>8.068</v>
+        <v>8.07</v>
       </c>
       <c r="AD5" s="4" t="n">
-        <v>10.815</v>
+        <v>10.81</v>
       </c>
       <c r="AE5" s="4" t="n">
-        <v>0.209</v>
+        <v>0.21</v>
       </c>
       <c r="AF5" s="4" t="n">
-        <v>32.065</v>
+        <v>32.07</v>
       </c>
       <c r="AG5" s="4" t="n">
-        <v>4.936</v>
+        <v>4.94</v>
       </c>
       <c r="AH5" s="4" t="n">
-        <v>10.236</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>40751.32638888889</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>10.03</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>28.99</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>23.88</v>
-      </c>
-      <c r="G6" s="4" t="n">
-        <v>10.48</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>40.87</v>
-      </c>
-      <c r="I6" s="4" t="n">
-        <v>16.34</v>
-      </c>
-      <c r="J6" s="4" t="n">
-        <v>7.44</v>
-      </c>
-      <c r="K6" s="4" t="n">
-        <v>11.17</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>11.93</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <v>12.35</v>
-      </c>
-      <c r="N6" s="4" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="O6" s="4" t="n">
-        <v>10.33</v>
-      </c>
-      <c r="P6" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="4" t="n">
-        <v>8.73</v>
-      </c>
-      <c r="R6" s="4" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="T6" s="4" t="n">
-        <v>152.78</v>
-      </c>
-      <c r="U6" s="4" t="n">
-        <v>29.43</v>
-      </c>
-      <c r="V6" s="4" t="n">
-        <v>9.619999999999999</v>
-      </c>
-      <c r="W6" s="4" t="n">
-        <v>19.69</v>
-      </c>
-      <c r="X6" s="4" t="n">
-        <v>10.72</v>
-      </c>
-      <c r="Y6" s="4" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="Z6" s="4" t="n">
-        <v>19.95</v>
-      </c>
-      <c r="AA6" s="4" t="n">
-        <v>8.57</v>
-      </c>
-      <c r="AB6" s="4" t="n">
-        <v>7.87</v>
-      </c>
-      <c r="AC6" s="4" t="n">
-        <v>9.24</v>
-      </c>
-      <c r="AD6" s="4" t="n">
-        <v>12.54</v>
-      </c>
-      <c r="AE6" s="4" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="AF6" s="4" t="n">
-        <v>37.07</v>
-      </c>
-      <c r="AG6" s="4" t="n">
-        <v>5.69</v>
-      </c>
-      <c r="AH6" s="4" t="n">
-        <v>12.01</v>
+        <v>10.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>